<commit_message>
Q&A màn hình cập nhật tờ khai thuế TTDB
</commit_message>
<xml_diff>
--- a/2015/201510/30_Q&A/[ASOFT-ACC]_Q&A.xlsx
+++ b/2015/201510/30_Q&A/[ASOFT-ACC]_Q&A.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\THUC TAP\Ex\30_Q&amp;A\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16965" windowHeight="7020" tabRatio="333"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="66">
   <si>
     <t>#</t>
   </si>
@@ -263,6 +268,12 @@
   </si>
   <si>
     <t>Em thấy trong tài liệu phân tích, khi check vào các ô Phụ thuộc mua vào bán ra thì sẽ enable cho nhập liệu các chỉ tiêu khác nhau bên dưới lưới. Em thấy bên mục kiểm tra dữ liệu nhập trong tài liệu thì có dòng nếu ChiTieu[40b] &lt;= [40a] thì báo lỗi. Nhưng bên danh sách các ô ChiTieu enable lên cho nhập liệu thì ko thấy có 2 ô này. Như vậy em nên enable 2 ô này  trong mọi trường hợp luôn phải không a?</t>
+  </si>
+  <si>
+    <t>Màn hình cập nhật tờ khai thuế TTDB</t>
+  </si>
+  <si>
+    <t>Đối với tờ khai tháng: Nếu là tờ khai lần đầu thì lúc đọc tờ khai sẽ load dữ liệu tờ khai tháng nào lên (Nếu lấy dữ liệu của tháng liền kề trước đó để load lên vậy lấy dữ liệu lần bổ sung cuối cùng của tháng đó load lên hay sao). Tương tự đối với tờ khai ngày phát sinh: Nếu khai lần đầu thì lúc đọc tờ khai sẽ load dữ liệu của ngày nào lên (Nếu lấy dữ liệu của ngày liền kề trước đó để load lên vậy dữ liệu cần lấy có phải là dữ liệu lần bổ sung cuối cùng của ngày đó load lên hay sao)</t>
   </si>
 </sst>
 </file>
@@ -584,6 +595,45 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -608,12 +658,6 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -625,39 +669,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -932,7 +943,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -942,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="12.75"/>
@@ -970,10 +981,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="33" customHeight="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="69"/>
+      <c r="B1" s="57"/>
       <c r="C1" s="1"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -1395,66 +1406,66 @@
       <c r="S11" s="36"/>
     </row>
     <row r="12" spans="1:19" s="3" customFormat="1" ht="13.5">
-      <c r="A12" s="72">
+      <c r="A12" s="60">
         <v>10</v>
       </c>
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="70" t="s">
+      <c r="C12" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="65"/>
+      <c r="D12" s="53"/>
       <c r="E12" s="29"/>
       <c r="F12" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="63"/>
-      <c r="H12" s="57">
+      <c r="G12" s="49"/>
+      <c r="H12" s="51">
         <v>42197</v>
       </c>
-      <c r="I12" s="65" t="s">
+      <c r="I12" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="67" t="s">
+      <c r="K12" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="L12" s="53"/>
-      <c r="M12" s="55"/>
-      <c r="N12" s="57">
+      <c r="L12" s="66"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="51">
         <v>42347</v>
       </c>
-      <c r="O12" s="59" t="s">
+      <c r="O12" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="P12" s="61" t="s">
+      <c r="P12" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="Q12" s="49"/>
+      <c r="Q12" s="62"/>
       <c r="R12" s="37"/>
-      <c r="S12" s="51"/>
+      <c r="S12" s="64"/>
     </row>
     <row r="13" spans="1:19" s="3" customFormat="1" ht="13.5">
-      <c r="A13" s="73"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="66"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="29"/>
       <c r="F13" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="64"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="66"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="56"/>
-      <c r="N13" s="58"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="62"/>
-      <c r="Q13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="54"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="69"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="71"/>
+      <c r="P13" s="73"/>
+      <c r="Q13" s="63"/>
       <c r="R13" s="37"/>
-      <c r="S13" s="52"/>
+      <c r="S13" s="65"/>
     </row>
     <row r="14" spans="1:19" s="3" customFormat="1" ht="25.5">
       <c r="A14" s="29">
@@ -1651,17 +1662,25 @@
       <c r="R18" s="37"/>
       <c r="S18" s="36"/>
     </row>
-    <row r="19" spans="1:19" s="3" customFormat="1" ht="13.5">
+    <row r="19" spans="1:19" s="3" customFormat="1" ht="63.75">
       <c r="A19" s="29"/>
       <c r="B19" s="30"/>
       <c r="C19" s="30"/>
       <c r="D19" s="29"/>
       <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
+      <c r="F19" s="29" t="s">
+        <v>64</v>
+      </c>
       <c r="G19" s="31"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="29"/>
-      <c r="K19" s="33"/>
+      <c r="H19" s="32">
+        <v>42675</v>
+      </c>
+      <c r="I19" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="L19" s="33"/>
       <c r="M19" s="34"/>
       <c r="N19" s="32"/>
@@ -2276,6 +2295,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="Q12:Q13"/>
+    <mergeCell ref="S12:S13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="I12:I13"/>
@@ -2285,13 +2311,6 @@
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="Q12:Q13"/>
-    <mergeCell ref="S12:S13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="P12:P13"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14:B48 B3:B12">

</xml_diff>